<commit_message>
changed class name & add static & changed excel
Changed the class name of each file for a bug
And
Add a static for fixing a bug
added one more colour in excel file for original data set query time
</commit_message>
<xml_diff>
--- a/Data Collection/execution_result.xlsx
+++ b/Data Collection/execution_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1000" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="90">
   <si>
     <t>Q5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>match(p:person) where (p.gender='Male' and p.age&gt;=0 and p.age&lt;=100) and (p.gender='Female' and p.age&gt;=0 and p.age&lt;=100) return p;</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -3700,10 +3703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3711,10 +3714,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="8" customWidth="1"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -3724,23 +3728,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3751,7 +3758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3762,7 +3769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3773,7 +3780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3784,7 +3791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -3795,7 +3802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -3806,7 +3813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3817,7 +3824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -3828,7 +3835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -3839,7 +3846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -3850,7 +3857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -3861,7 +3868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -3872,7 +3879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -3883,7 +3890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -3894,7 +3901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -4957,10 +4964,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4968,10 +4975,12 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="8" customWidth="1"/>
+    <col min="5" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -4981,23 +4990,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -5008,7 +5020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -5019,7 +5031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -5030,7 +5042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -5041,7 +5053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -5052,7 +5064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -5063,7 +5075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -5074,7 +5086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -5085,7 +5097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -5107,7 +5119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -5118,7 +5130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -5129,7 +5141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -5140,7 +5152,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -5151,7 +5163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -6213,10 +6225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6224,10 +6236,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="8" customWidth="1"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -6237,23 +6250,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -6264,7 +6280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -6275,7 +6291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -6286,7 +6302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -6297,7 +6313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -6308,7 +6324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -6319,7 +6335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -6330,7 +6346,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -6341,7 +6357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -6352,7 +6368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -6363,7 +6379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -6374,7 +6390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -6385,7 +6401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -6396,7 +6412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -6407,7 +6423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -7469,10 +7485,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7480,10 +7496,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -7493,23 +7510,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -7520,7 +7540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -7531,7 +7551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -7542,7 +7562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -7553,7 +7573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -7564,7 +7584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -7575,7 +7595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -7586,7 +7606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -7597,7 +7617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -7608,7 +7628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -7619,7 +7639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -7630,7 +7650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -7641,7 +7661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -7652,7 +7672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -7663,7 +7683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -8725,10 +8745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8736,10 +8756,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -8749,23 +8770,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -8776,7 +8800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -8787,7 +8811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -8798,7 +8822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -8809,7 +8833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -8820,7 +8844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -8831,7 +8855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -8842,7 +8866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -8853,7 +8877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -8864,7 +8888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -8875,7 +8899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -8886,7 +8910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -8897,7 +8921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -8908,7 +8932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -8919,7 +8943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -9981,10 +10005,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9992,10 +10016,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -10005,23 +10030,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -10032,7 +10060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -10043,7 +10071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -10054,7 +10082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -10065,7 +10093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -10076,7 +10104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -10087,7 +10115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -10098,7 +10126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -10109,7 +10137,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -10120,7 +10148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -10131,7 +10159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -10142,7 +10170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -10153,7 +10181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -10164,7 +10192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -10175,7 +10203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -11237,10 +11265,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11248,10 +11276,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -11261,23 +11290,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -11288,7 +11320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -11299,7 +11331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -11310,7 +11342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -11321,7 +11353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -11332,7 +11364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -11343,7 +11375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -11354,7 +11386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -11365,7 +11397,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -11376,7 +11408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -11387,7 +11419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -11398,7 +11430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -11409,7 +11441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -11420,7 +11452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -11431,7 +11463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -12493,10 +12525,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12504,10 +12536,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -12517,23 +12550,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -12544,7 +12580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -12555,7 +12591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -12566,7 +12602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -12577,7 +12613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -12588,7 +12624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -12599,7 +12635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -12610,7 +12646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -12621,7 +12657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -12632,7 +12668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -12643,7 +12679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -12654,7 +12690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -12665,7 +12701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -12676,7 +12712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -12687,7 +12723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -13749,10 +13785,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13760,10 +13796,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8"/>
+    <col min="5" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -13773,23 +13810,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -13800,7 +13840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -13811,7 +13851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -13822,7 +13862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -13833,7 +13873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -13844,7 +13884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -13855,7 +13895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -13866,7 +13906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -13877,7 +13917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -13888,7 +13928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -13899,7 +13939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -13910,7 +13950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -13921,7 +13961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -13932,7 +13972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -13943,7 +13983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>
@@ -15005,10 +15045,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15016,10 +15056,11 @@
     <col min="1" max="1" width="7" style="8" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.83203125" customWidth="1"/>
+    <col min="4" max="8" width="11.83203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -15029,23 +15070,26 @@
       <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -15056,7 +15100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -15067,7 +15111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -15078,7 +15122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -15089,7 +15133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -15100,7 +15144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -15111,7 +15155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -15122,7 +15166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -15133,7 +15177,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -15144,7 +15188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -15155,7 +15199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -15166,7 +15210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -15177,7 +15221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -15188,7 +15232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>2</v>
       </c>
@@ -15199,7 +15243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>3</v>
       </c>

</xml_diff>